<commit_message>
Write up completed and saved as pdf
</commit_message>
<xml_diff>
--- a/Graphics/table1.xlsx
+++ b/Graphics/table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6da0f05bc4637dcc/Documents/Masters 2021-22/CEGE0042 Spatio-Temporal Data Analysis and Data Mining/Coursework/STDM-coursework/Graphics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{4D1964D2-23AC-475A-9056-EC33F0B3262C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74DB1009-A544-4A17-9EFD-C846A774ABD0}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{4D1964D2-23AC-475A-9056-EC33F0B3262C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5B4346-767E-45FE-8D6F-D8B20DEA4AAA}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="720" windowWidth="19992" windowHeight="11172" xr2:uid="{7782B79B-9EF4-4741-8847-F4E314404DCF}"/>
+    <workbookView xWindow="28680" yWindow="-5550" windowWidth="29040" windowHeight="15840" xr2:uid="{7782B79B-9EF4-4741-8847-F4E314404DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Model</t>
   </si>
@@ -95,12 +95,18 @@
   </si>
   <si>
     <t>fit8.Ar</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -308,11 +314,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="medium">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="medium">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -352,6 +408,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD100728-DE4F-4690-9175-CEE2C209D6A9}">
-  <dimension ref="A2:J28"/>
+  <dimension ref="A2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F11"/>
+      <selection activeCell="B3" sqref="B3:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,11 +750,12 @@
     <col min="3" max="3" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -694,11 +766,14 @@
       <c r="E3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
@@ -711,11 +786,14 @@
       <c r="E4" s="11">
         <v>23637.25</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="18">
+        <v>0.84563999999999995</v>
+      </c>
+      <c r="G4" s="12">
         <v>0.54259999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -729,15 +807,18 @@
       <c r="E5" s="4">
         <v>23639.23</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="19">
+        <v>0.84562999999999999</v>
+      </c>
+      <c r="G5" s="5">
         <v>0.42880000000000001</v>
       </c>
-      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="6" t="s">
         <v>14</v>
@@ -751,15 +832,18 @@
       <c r="E6" s="4">
         <v>23635.58</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="19">
+        <v>0.84484000000000004</v>
+      </c>
+      <c r="G6" s="5">
         <v>0.41120000000000001</v>
       </c>
-      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -773,15 +857,18 @@
       <c r="E7" s="4">
         <v>23634.17</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="19">
+        <v>0.84411999999999998</v>
+      </c>
+      <c r="G7" s="5">
         <v>0.29249999999999998</v>
       </c>
-      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="6" t="s">
         <v>16</v>
@@ -795,15 +882,18 @@
       <c r="E8" s="4">
         <v>23636.11</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="19">
+        <v>0.84408000000000005</v>
+      </c>
+      <c r="G8" s="5">
         <v>0.1938</v>
       </c>
-      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="6" t="s">
         <v>17</v>
@@ -817,15 +907,18 @@
       <c r="E9" s="4">
         <v>23634.16</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="21">
+        <v>0.84409999999999996</v>
+      </c>
+      <c r="G9" s="5">
         <v>0.27329999999999999</v>
       </c>
-      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="6" t="s">
         <v>18</v>
@@ -839,15 +932,18 @@
       <c r="E10" s="4">
         <v>23637.34</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="19">
+        <v>0.84563999999999995</v>
+      </c>
+      <c r="G10" s="5">
         <v>0.51729999999999998</v>
       </c>
-      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="7" t="s">
         <v>19</v>
@@ -861,217 +957,237 @@
       <c r="E11" s="8">
         <v>23635.66</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="20">
+        <v>0.84484000000000004</v>
+      </c>
+      <c r="G11" s="9">
         <v>0.3826</v>
       </c>
-      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="2"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="2"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="2"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="2"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="2"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="2"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="2"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>